<commit_message>
Separated Android and Telegram bot
</commit_message>
<xml_diff>
--- a/actions/student_db_new.xlsx
+++ b/actions/student_db_new.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>User</t>
   </si>
@@ -55,13 +55,7 @@
     <t>Other</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>zyx</t>
-  </si>
-  <si>
-    <t>1082171472</t>
+    <t>test1</t>
   </si>
 </sst>
 </file>
@@ -419,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,11 +461,11 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2">
+        <v>1082171472</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -489,10 +483,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -509,7 +503,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -530,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -545,47 +539,6 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
         <v>0</v>
       </c>
     </row>

</xml_diff>